<commit_message>
Added PDF extraction and updated navigation bar
</commit_message>
<xml_diff>
--- a/feature_progress_tracking.xlsx
+++ b/feature_progress_tracking.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Morgan\Documents\Aberystwyth University\Year 4_2nd\Major Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{B0209944-4152-456D-8512-84651CD37F90}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B92916E-1618-405E-86AD-D34F901A4705}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={94923ADF-2239-4D97-991A-C1D9A83B20C5}</author>
     <author>tc={493DB784-7020-4B17-8C09-3B86F42D0599}</author>
   </authors>
   <commentList>
-    <comment ref="J7" authorId="0" shapeId="0">
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -45,7 +45,7 @@
     Design is emerging from the refactorings. It is being generated from the code at the end. With changes made to the hogh-level design by hand if needed.</t>
       </text>
     </comment>
-    <comment ref="W14" authorId="1" shapeId="0">
+    <comment ref="W14" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Design</t>
   </si>
@@ -142,13 +142,16 @@
   </si>
   <si>
     <t>Search the list/category of sessions for a session with a specific title or date</t>
+  </si>
+  <si>
+    <t>Add extratcion from uploaded pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,18 +195,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -296,9 +287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -321,23 +309,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -674,11 +665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G4:Y31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="G4:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Y30" sqref="Y30"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +680,7 @@
     <col min="11" max="11" width="16.28515625" customWidth="1"/>
     <col min="12" max="12" width="22.28515625" customWidth="1"/>
     <col min="13" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="22.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.85546875" style="6" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="45.42578125" style="5" customWidth="1"/>
     <col min="17" max="24" width="15.7109375" customWidth="1"/>
     <col min="25" max="25" width="61" bestFit="1" customWidth="1"/>
@@ -764,35 +755,35 @@
       </c>
     </row>
     <row r="14" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="O14" s="17" t="s">
+      <c r="O14" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="P14" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="6" t="s">
+      <c r="Q14" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6" t="s">
+      <c r="R14" s="18"/>
+      <c r="S14" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6" t="s">
+      <c r="T14" s="18"/>
+      <c r="U14" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="V14" s="6"/>
-      <c r="W14" s="6" t="s">
+      <c r="V14" s="18"/>
+      <c r="W14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6" t="s">
+      <c r="X14" s="18"/>
+      <c r="Y14" s="18" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="7:25" x14ac:dyDescent="0.25">
-      <c r="O15" s="17"/>
-      <c r="P15" s="15"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="20"/>
       <c r="Q15" s="3" t="s">
         <v>10</v>
       </c>
@@ -817,205 +808,230 @@
       <c r="X15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Y15" s="6"/>
+      <c r="Y15" s="18"/>
     </row>
     <row r="16" spans="7:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="O16" s="8" t="s">
+      <c r="O16" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="9" t="s">
+      <c r="P16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q16" s="10">
+      <c r="Q16" s="9">
         <v>43516</v>
       </c>
-      <c r="R16" s="10">
+      <c r="R16" s="9">
         <v>43516</v>
       </c>
-      <c r="S16" s="11">
+      <c r="S16" s="10">
         <v>43520</v>
       </c>
-      <c r="T16" s="11">
+      <c r="T16" s="10">
         <v>43522</v>
       </c>
-      <c r="U16" s="11">
+      <c r="U16" s="10">
         <v>43523</v>
       </c>
-      <c r="V16" s="11">
+      <c r="V16" s="10">
         <v>43497</v>
       </c>
-      <c r="W16" s="11">
+      <c r="W16" s="10">
         <v>43523</v>
       </c>
-      <c r="X16" s="11">
+      <c r="X16" s="10">
         <v>43497</v>
       </c>
-      <c r="Y16" s="13" t="s">
+      <c r="Y16" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="15:25" x14ac:dyDescent="0.25">
-      <c r="O17" s="12" t="s">
+      <c r="O17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P17" s="16" t="s">
+      <c r="P17" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="10" t="s">
+      <c r="Q17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="R17" s="10">
+      <c r="R17" s="9">
         <v>43525</v>
       </c>
-      <c r="S17" s="10" t="s">
+      <c r="S17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="T17" s="10">
+      <c r="T17" s="9">
         <v>43525</v>
       </c>
-      <c r="U17" s="10" t="s">
+      <c r="U17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="V17" s="10">
+      <c r="V17" s="9">
         <v>43525</v>
       </c>
-      <c r="W17" s="10" t="s">
+      <c r="W17" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="X17" s="10">
+      <c r="X17" s="9">
         <v>43525</v>
       </c>
-      <c r="Y17" s="14" t="s">
+      <c r="Y17" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="15:25" x14ac:dyDescent="0.25">
-      <c r="O18" s="18" t="s">
+      <c r="O18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P18" s="19" t="s">
+      <c r="P18" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="17">
         <v>43527</v>
       </c>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20">
+      <c r="R18" s="17"/>
+      <c r="S18" s="17">
         <v>43527</v>
       </c>
-      <c r="T18" s="18"/>
-      <c r="U18" s="20">
+      <c r="T18" s="15"/>
+      <c r="U18" s="17">
         <v>43527</v>
       </c>
-      <c r="V18" s="18"/>
-      <c r="W18" s="20">
+      <c r="V18" s="15"/>
+      <c r="W18" s="17">
         <v>43527</v>
       </c>
-      <c r="X18" s="18"/>
-      <c r="Y18" s="13"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="12"/>
     </row>
     <row r="19" spans="15:25" x14ac:dyDescent="0.25">
-      <c r="O19" s="18" t="s">
+      <c r="O19" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19" s="17">
+        <v>43529</v>
+      </c>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17">
+        <v>43529</v>
+      </c>
+      <c r="T19" s="15"/>
+      <c r="U19" s="17">
+        <v>43529</v>
+      </c>
+      <c r="V19" s="15"/>
+      <c r="W19" s="17">
+        <v>43529</v>
+      </c>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="12"/>
+    </row>
+    <row r="20" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="Q20" s="17">
         <v>43528</v>
       </c>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20">
+      <c r="R20" s="17"/>
+      <c r="S20" s="17">
         <v>43528</v>
       </c>
-      <c r="T19" s="18"/>
-      <c r="U19" s="20">
+      <c r="T20" s="15"/>
+      <c r="U20" s="17">
         <v>43528</v>
       </c>
-      <c r="V19" s="18"/>
-      <c r="W19" s="20">
+      <c r="V20" s="15"/>
+      <c r="W20" s="17">
         <v>43528</v>
       </c>
-      <c r="X19" s="18"/>
-      <c r="Y19" s="13"/>
-    </row>
-    <row r="20" spans="15:25" x14ac:dyDescent="0.25">
-      <c r="O20" s="18" t="s">
+      <c r="X20" s="15"/>
+      <c r="Y20" s="12"/>
+    </row>
+    <row r="21" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O21" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P20" s="19" t="s">
+      <c r="P21" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="Q20" s="20">
+      <c r="Q21" s="17">
         <v>43528</v>
       </c>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20">
+      <c r="R21" s="17"/>
+      <c r="S21" s="17">
         <v>43528</v>
       </c>
-      <c r="T20" s="18"/>
-      <c r="U20" s="20">
+      <c r="T21" s="15"/>
+      <c r="U21" s="17">
         <v>43528</v>
       </c>
-      <c r="V20" s="18"/>
-      <c r="W20" s="20">
+      <c r="V21" s="15"/>
+      <c r="W21" s="17">
         <v>43528</v>
       </c>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="13"/>
-    </row>
-    <row r="21" spans="15:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="O21" s="18" t="s">
+      <c r="X21" s="15"/>
+      <c r="Y21" s="12"/>
+    </row>
+    <row r="22" spans="15:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="O22" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P21" s="19" t="s">
+      <c r="P22" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q22" s="17">
         <v>43529</v>
       </c>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20">
+      <c r="R22" s="17"/>
+      <c r="S22" s="17">
         <v>43529</v>
       </c>
-      <c r="T21" s="18"/>
-      <c r="U21" s="20">
+      <c r="T22" s="15"/>
+      <c r="U22" s="17">
         <v>43529</v>
       </c>
-      <c r="V21" s="18"/>
-      <c r="W21" s="20">
+      <c r="V22" s="15"/>
+      <c r="W22" s="17">
         <v>43529</v>
       </c>
-      <c r="X21" s="18"/>
-      <c r="Y21" s="13"/>
-    </row>
-    <row r="22" spans="15:25" x14ac:dyDescent="0.25">
-      <c r="O22" s="18" t="s">
+      <c r="X22" s="15"/>
+      <c r="Y22" s="12"/>
+    </row>
+    <row r="23" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="O23" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="P22" s="19" t="s">
+      <c r="P23" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q23" s="17">
         <v>43530</v>
       </c>
-      <c r="R22" s="18"/>
-      <c r="S22" s="20">
+      <c r="R23" s="15"/>
+      <c r="S23" s="17">
         <v>43530</v>
       </c>
-      <c r="T22" s="18"/>
-      <c r="U22" s="20">
+      <c r="T23" s="15"/>
+      <c r="U23" s="17">
         <v>43530</v>
       </c>
-      <c r="V22" s="18"/>
-      <c r="W22" s="20">
+      <c r="V23" s="15"/>
+      <c r="W23" s="17">
         <v>43530</v>
       </c>
-      <c r="X22" s="18"/>
-      <c r="Y22" s="13"/>
-    </row>
-    <row r="31" spans="15:25" x14ac:dyDescent="0.25">
-      <c r="R31" s="5"/>
+      <c r="X23" s="15"/>
+      <c r="Y23" s="12"/>
+    </row>
+    <row r="32" spans="15:25" x14ac:dyDescent="0.25">
+      <c r="R32" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>